<commit_message>
importação com separador funcionando
</commit_message>
<xml_diff>
--- a/AfincoApp/uploads/import.xlsx
+++ b/AfincoApp/uploads/import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBB861F-EDBD-46B8-A4C6-092F894DD30B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{09C906E2-377B-41D4-B890-2055D0F3005A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{974D8A04-0931-412F-9F5F-6D146D5FF38B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3CA86AC0-5B60-456C-B6AD-089B8CA1E9F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,20 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>1520; 1595.6666; 2555</t>
+  </si>
+  <si>
+    <t>1588,636; eyerte; 52525</t>
+  </si>
+  <si>
+    <t>62626,5; 5858; 222</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -66,9 +80,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,46 +395,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E5CCD6E-D5EB-4C2E-8254-A0EF27FDDB1B}">
-  <dimension ref="A1:A6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{478C2BB5-06D6-4268-849B-21171DF1406A}">
+  <dimension ref="A1:A3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.77734375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>3210</v>
+      <c r="A1" t="s">
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>-666</v>
+      <c r="A2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
-        <v>-36.252499999999998</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>141415</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>626066</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>88.000000499999999</v>
+      <c r="A3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>